<commit_message>
Complete new DataBase + follow fixes
</commit_message>
<xml_diff>
--- a/Work/Data/db.xlsx
+++ b/Work/Data/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\PyProject\python_project_192\Work\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2E3917-2303-434F-958A-29A02E6DEE2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FEF909-85C5-401E-B098-82EC63EC9DED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{3E971001-3800-4193-8498-245E767CB2F4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3E971001-3800-4193-8498-245E767CB2F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Учет" sheetId="1" r:id="rId1"/>
@@ -104,21 +104,6 @@
     <t>Бухгалтер</t>
   </si>
   <si>
-    <t>Логистика</t>
-  </si>
-  <si>
-    <t>Бухгалтерия</t>
-  </si>
-  <si>
-    <t>Отдел кадров</t>
-  </si>
-  <si>
-    <t>Отдел продаж</t>
-  </si>
-  <si>
-    <t>Кредитование</t>
-  </si>
-  <si>
     <t>Павлов Евдоким Валерьянович</t>
   </si>
   <si>
@@ -834,13 +819,28 @@
   </si>
   <si>
     <t>Осипова Алена Ивановна</t>
+  </si>
+  <si>
+    <t>Техническая поддержка</t>
+  </si>
+  <si>
+    <t>Аналитика</t>
+  </si>
+  <si>
+    <t>Разработка</t>
+  </si>
+  <si>
+    <t>Контроль качества</t>
+  </si>
+  <si>
+    <t>Обучение</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -849,13 +849,63 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE028CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -885,7 +935,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -902,12 +952,25 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE028CE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1216,10 +1279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802CA84B-12BF-4C23-A805-60116DA63581}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1229,14 +1292,15 @@
     <col min="3" max="3" width="15.54296875" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
     <col min="5" max="5" width="18" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1247,8 +1311,9 @@
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1259,13 +1324,14 @@
         <v>27</v>
       </c>
       <c r="D2">
-        <v>120800</v>
+        <v>60400</v>
       </c>
       <c r="E2">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <f t="shared" ref="A3:A34" si="0">A2+1</f>
         <v>2</v>
@@ -1276,14 +1342,16 @@
       <c r="C3">
         <v>24</v>
       </c>
-      <c r="D3">
-        <v>79120</v>
+      <c r="D3" s="14">
+        <v>49410</v>
       </c>
       <c r="E3">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="7"/>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1295,13 +1363,15 @@
         <v>27</v>
       </c>
       <c r="D4">
-        <v>290400</v>
+        <v>145200</v>
       </c>
       <c r="E4">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="7"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1313,13 +1383,14 @@
         <v>19</v>
       </c>
       <c r="D5">
-        <v>277200</v>
+        <v>138600</v>
       </c>
       <c r="E5">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1330,14 +1401,15 @@
       <c r="C6">
         <v>17</v>
       </c>
-      <c r="D6">
-        <v>99760</v>
+      <c r="D6" s="15">
+        <v>60480</v>
       </c>
       <c r="E6">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1349,13 +1421,15 @@
         <v>30</v>
       </c>
       <c r="D7">
-        <v>174000</v>
+        <v>87000</v>
       </c>
       <c r="E7">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="7"/>
+      <c r="L7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1367,13 +1441,15 @@
         <v>19</v>
       </c>
       <c r="D8">
-        <v>107200</v>
+        <v>53600</v>
       </c>
       <c r="E8">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="7"/>
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1385,13 +1461,14 @@
         <v>24</v>
       </c>
       <c r="D9">
-        <v>102400</v>
+        <v>51200</v>
       </c>
       <c r="E9">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1403,13 +1480,14 @@
         <v>20</v>
       </c>
       <c r="D10">
-        <v>186000</v>
+        <v>93000</v>
       </c>
       <c r="E10">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1420,14 +1498,15 @@
       <c r="C11">
         <v>25</v>
       </c>
-      <c r="D11">
-        <v>60200</v>
+      <c r="D11" s="13">
+        <v>36950</v>
       </c>
       <c r="E11">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1438,14 +1517,15 @@
       <c r="C12">
         <v>28</v>
       </c>
-      <c r="D12">
-        <v>60200</v>
+      <c r="D12" s="13">
+        <v>33500</v>
       </c>
       <c r="E12">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1456,14 +1536,15 @@
       <c r="C13">
         <v>19</v>
       </c>
-      <c r="D13">
-        <v>99760</v>
+      <c r="D13" s="15">
+        <v>55230</v>
       </c>
       <c r="E13">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1475,13 +1556,14 @@
         <v>22</v>
       </c>
       <c r="D14">
-        <v>107800</v>
+        <v>53900</v>
       </c>
       <c r="E14">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1493,13 +1575,14 @@
         <v>22</v>
       </c>
       <c r="D15">
-        <v>100800</v>
+        <v>50400</v>
       </c>
       <c r="E15">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1511,13 +1594,14 @@
         <v>27</v>
       </c>
       <c r="D16">
-        <v>93100</v>
+        <v>46550</v>
       </c>
       <c r="E16">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1528,14 +1612,15 @@
       <c r="C17">
         <v>26</v>
       </c>
-      <c r="D17">
-        <v>99760</v>
+      <c r="D17" s="15">
+        <v>68180</v>
       </c>
       <c r="E17">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1546,14 +1631,15 @@
       <c r="C18">
         <v>27</v>
       </c>
-      <c r="D18">
-        <v>86000</v>
+      <c r="D18" s="12">
+        <v>62100</v>
       </c>
       <c r="E18">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1565,13 +1651,14 @@
         <v>16</v>
       </c>
       <c r="D19">
-        <v>91000</v>
+        <v>45500</v>
       </c>
       <c r="E19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1583,13 +1670,14 @@
         <v>17</v>
       </c>
       <c r="D20">
-        <v>187000</v>
+        <v>93500</v>
       </c>
       <c r="E20">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1601,13 +1689,14 @@
         <v>17</v>
       </c>
       <c r="D21">
-        <v>252000</v>
+        <v>126000</v>
       </c>
       <c r="E21">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1619,13 +1708,14 @@
         <v>29</v>
       </c>
       <c r="D22">
-        <v>254400</v>
+        <v>127200</v>
       </c>
       <c r="E22">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1636,14 +1726,15 @@
       <c r="C23">
         <v>26</v>
       </c>
-      <c r="D23">
-        <v>79120</v>
+      <c r="D23" s="14">
+        <v>43210</v>
       </c>
       <c r="E23">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1654,14 +1745,15 @@
       <c r="C24">
         <v>22</v>
       </c>
-      <c r="D24">
-        <v>99760</v>
+      <c r="D24" s="15">
+        <v>64780</v>
       </c>
       <c r="E24">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1672,14 +1764,15 @@
       <c r="C25">
         <v>15</v>
       </c>
-      <c r="D25">
-        <v>8600</v>
+      <c r="D25" s="12">
+        <v>44200</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1690,14 +1783,15 @@
       <c r="C26">
         <v>23</v>
       </c>
-      <c r="D26">
-        <v>481600</v>
+      <c r="D26" s="11">
+        <v>177750</v>
       </c>
       <c r="E26">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1709,13 +1803,14 @@
         <v>23</v>
       </c>
       <c r="D27">
-        <v>112800</v>
+        <v>56400</v>
       </c>
       <c r="E27">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1727,13 +1822,14 @@
         <v>24</v>
       </c>
       <c r="D28">
-        <v>88900</v>
+        <v>44450</v>
       </c>
       <c r="E28">
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1744,14 +1840,15 @@
       <c r="C29">
         <v>18</v>
       </c>
-      <c r="D29">
-        <v>292400</v>
+      <c r="D29" s="10">
+        <v>139150</v>
       </c>
       <c r="E29">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1762,14 +1859,15 @@
       <c r="C30">
         <v>17</v>
       </c>
-      <c r="D30">
-        <v>8600</v>
+      <c r="D30" s="12">
+        <v>47570</v>
       </c>
       <c r="E30">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1780,14 +1878,15 @@
       <c r="C31">
         <v>17</v>
       </c>
-      <c r="D31">
-        <v>481600</v>
+      <c r="D31" s="11">
+        <v>156850</v>
       </c>
       <c r="E31">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1799,13 +1898,14 @@
         <v>15</v>
       </c>
       <c r="D32">
-        <v>175000</v>
+        <v>87500</v>
       </c>
       <c r="E32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1816,14 +1916,15 @@
       <c r="C33">
         <v>18</v>
       </c>
-      <c r="D33">
-        <v>99760</v>
+      <c r="D33" s="15">
+        <v>51530</v>
       </c>
       <c r="E33">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1835,13 +1936,14 @@
         <v>19</v>
       </c>
       <c r="D34">
-        <v>256800</v>
+        <v>128400</v>
       </c>
       <c r="E34">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" ref="A35:A51" si="1">A34+1</f>
         <v>34</v>
@@ -1852,14 +1954,15 @@
       <c r="C35">
         <v>16</v>
       </c>
-      <c r="D35">
-        <v>292400</v>
+      <c r="D35" s="10">
+        <v>156800</v>
       </c>
       <c r="E35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -1870,14 +1973,15 @@
       <c r="C36">
         <v>27</v>
       </c>
-      <c r="D36">
-        <v>79120</v>
+      <c r="D36" s="14">
+        <v>54060</v>
       </c>
       <c r="E36">
         <v>46</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -1888,14 +1992,15 @@
       <c r="C37">
         <v>27</v>
       </c>
-      <c r="D37">
-        <v>292400</v>
+      <c r="D37" s="10">
+        <v>142600</v>
       </c>
       <c r="E37">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -1906,14 +2011,15 @@
       <c r="C38">
         <v>19</v>
       </c>
-      <c r="D38">
-        <v>292400</v>
+      <c r="D38" s="10">
+        <v>145750</v>
       </c>
       <c r="E38">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -1924,14 +2030,15 @@
       <c r="C39">
         <v>30</v>
       </c>
-      <c r="D39">
-        <v>60200</v>
+      <c r="D39" s="13">
+        <v>50050</v>
       </c>
       <c r="E39">
         <v>50</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -1942,14 +2049,15 @@
       <c r="C40">
         <v>23</v>
       </c>
-      <c r="D40">
-        <v>60200</v>
+      <c r="D40" s="13">
+        <v>45650</v>
       </c>
       <c r="E40">
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -1960,14 +2068,15 @@
       <c r="C41">
         <v>17</v>
       </c>
-      <c r="D41">
-        <v>292400</v>
+      <c r="D41" s="10">
+        <v>159600</v>
       </c>
       <c r="E41">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -1978,14 +2087,15 @@
       <c r="C42">
         <v>22</v>
       </c>
-      <c r="D42">
-        <v>481600</v>
+      <c r="D42" s="11">
+        <v>172350</v>
       </c>
       <c r="E42">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -1996,14 +2106,15 @@
       <c r="C43">
         <v>25</v>
       </c>
-      <c r="D43">
-        <v>79120</v>
+      <c r="D43" s="14">
+        <v>58660</v>
       </c>
       <c r="E43">
         <v>37</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -2014,14 +2125,15 @@
       <c r="C44">
         <v>21</v>
       </c>
-      <c r="D44">
-        <v>86000</v>
+      <c r="D44" s="12">
+        <v>57800</v>
       </c>
       <c r="E44">
         <v>25</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -2032,14 +2144,15 @@
       <c r="C45">
         <v>19</v>
       </c>
-      <c r="D45">
-        <v>481600</v>
+      <c r="D45" s="11">
+        <v>163600</v>
       </c>
       <c r="E45">
         <v>18</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -2051,13 +2164,14 @@
         <v>17</v>
       </c>
       <c r="D46">
-        <v>92400</v>
+        <v>46200</v>
       </c>
       <c r="E46">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -2068,14 +2182,15 @@
       <c r="C47">
         <v>16</v>
       </c>
-      <c r="D47">
-        <v>86000</v>
+      <c r="D47" s="12">
+        <v>51600</v>
       </c>
       <c r="E47">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -2086,14 +2201,15 @@
       <c r="C48">
         <v>20</v>
       </c>
-      <c r="D48">
-        <v>481600</v>
+      <c r="D48" s="11">
+        <v>160600</v>
       </c>
       <c r="E48">
         <v>24</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -2104,14 +2220,15 @@
       <c r="C49">
         <v>18</v>
       </c>
-      <c r="D49">
-        <v>60200</v>
+      <c r="D49" s="13">
+        <v>40350</v>
       </c>
       <c r="E49">
         <v>13</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -2123,13 +2240,14 @@
         <v>19</v>
       </c>
       <c r="D50">
-        <v>177000</v>
+        <v>88500</v>
       </c>
       <c r="E50">
         <v>21</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -2140,12 +2258,13 @@
       <c r="C51">
         <v>27</v>
       </c>
-      <c r="D51">
-        <v>79120</v>
+      <c r="D51" s="14">
+        <v>41210</v>
       </c>
       <c r="E51">
         <v>45</v>
       </c>
+      <c r="F51" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E51" xr:uid="{3AB0C455-E0A1-4208-8A7E-BDFA1C3E7149}"/>
@@ -2153,16 +2272,16 @@
     <sortCondition ref="F2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E65D3C7-96B9-4249-84BC-8FFE97811FCF}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2184,7 +2303,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
       <c r="B2">
@@ -2196,7 +2315,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A34" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3">
@@ -2207,8 +2326,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
-        <f>A3+1</f>
+      <c r="A4" s="12">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4">
@@ -2219,8 +2338,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <f>A4+1</f>
+      <c r="A5" s="10">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5">
@@ -2231,8 +2350,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
-        <f>A5+1</f>
+      <c r="A6" s="9">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6">
@@ -2243,8 +2362,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
-        <f>A6+1</f>
+      <c r="A7" s="12">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7">
@@ -2255,8 +2374,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
-        <f>A7+1</f>
+      <c r="A8" s="10">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8">
@@ -2267,8 +2386,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
-        <f>A8+1</f>
+      <c r="A9" s="11">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9">
@@ -2280,7 +2399,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10">
@@ -2292,7 +2411,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <f>A10+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11">
@@ -2304,7 +2423,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12">
@@ -2315,8 +2434,8 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
-        <f>A12+1</f>
+      <c r="A13" s="15">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13">
@@ -2327,8 +2446,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
-        <f>A13+1</f>
+      <c r="A14" s="13">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14">
@@ -2339,8 +2458,8 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
-        <f>A14+1</f>
+      <c r="A15" s="10">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15">
@@ -2351,8 +2470,8 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
-        <f>A15+1</f>
+      <c r="A16" s="15">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16">
@@ -2362,9 +2481,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <f>A16+1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17">
@@ -2374,9 +2493,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
-        <f>A17+1</f>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="15">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18">
@@ -2386,9 +2505,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
-        <f>A18+1</f>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="11">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19">
@@ -2398,9 +2517,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <f>A19+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20">
@@ -2410,9 +2529,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <f>A20+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21">
@@ -2422,9 +2541,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
-        <f>A21+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22">
@@ -2433,10 +2552,11 @@
       <c r="C22" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="4">
-        <f>A22+1</f>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="10">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23">
@@ -2446,9 +2566,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
-        <f>A23+1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24">
@@ -2458,9 +2578,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="4">
-        <f>A24+1</f>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="11">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25">
@@ -2470,9 +2590,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="4">
-        <f>A25+1</f>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="12">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26">
@@ -2482,9 +2602,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="4">
-        <f>A26+1</f>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="15">
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27">
@@ -2494,9 +2614,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="4">
-        <f>A27+1</f>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="11">
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28">
@@ -2506,9 +2626,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
-        <f>A28+1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29">
@@ -2518,9 +2638,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
-        <f>A29+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30">
@@ -2530,9 +2650,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="4">
-        <f>A30+1</f>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="11">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31">
@@ -2542,9 +2662,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
-        <f>A31+1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32">
@@ -2555,8 +2675,8 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="4">
-        <f>A32+1</f>
+      <c r="A33" s="13">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33">
@@ -2567,8 +2687,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="4">
-        <f>A33+1</f>
+      <c r="A34" s="14">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B34">
@@ -2580,7 +2700,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
-        <f>A34+1</f>
+        <f t="shared" ref="A35:A51" si="1">A34+1</f>
         <v>34</v>
       </c>
       <c r="B35">
@@ -2592,7 +2712,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
-        <f>A35+1</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36">
@@ -2603,8 +2723,8 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="4">
-        <f>A36+1</f>
+      <c r="A37" s="13">
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37">
@@ -2615,8 +2735,8 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="4">
-        <f>A37+1</f>
+      <c r="A38" s="14">
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38">
@@ -2627,8 +2747,8 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="4">
-        <f>A38+1</f>
+      <c r="A39" s="15">
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39">
@@ -2639,8 +2759,8 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="4">
-        <f>A39+1</f>
+      <c r="A40" s="14">
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40">
@@ -2651,8 +2771,8 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="4">
-        <f>A40+1</f>
+      <c r="A41" s="10">
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41">
@@ -2664,7 +2784,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
-        <f>A41+1</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42">
@@ -2676,7 +2796,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
-        <f>A42+1</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43">
@@ -2688,7 +2808,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
-        <f>A43+1</f>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44">
@@ -2699,8 +2819,8 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="4">
-        <f>A44+1</f>
+      <c r="A45" s="12">
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45">
@@ -2711,8 +2831,8 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="4">
-        <f>A45+1</f>
+      <c r="A46" s="14">
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B46">
@@ -2724,7 +2844,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
-        <f>A46+1</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B47">
@@ -2735,8 +2855,8 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="4">
-        <f>A47+1</f>
+      <c r="A48" s="13">
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B48">
@@ -2748,7 +2868,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
-        <f>A48+1</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49">
@@ -2760,7 +2880,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
-        <f>A49+1</f>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50">
@@ -2771,8 +2891,8 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="4">
-        <f>A50+1</f>
+      <c r="A51" s="13">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51">
@@ -2785,6 +2905,7 @@
   </sheetData>
   <autoFilter ref="A1:C51" xr:uid="{FD4CF48E-A833-48FB-BC6A-33F9A826F478}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2793,7 +2914,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2812,7 +2933,7 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -2829,7 +2950,7 @@
         <v>172</v>
       </c>
       <c r="D2">
-        <v>2800</v>
+        <v>900</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -2841,13 +2962,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C3">
         <v>172</v>
       </c>
       <c r="D3">
-        <v>1700</v>
+        <v>800</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -2864,10 +2985,10 @@
         <v>172</v>
       </c>
       <c r="D4">
-        <v>350</v>
+        <v>175</v>
       </c>
       <c r="E4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -2881,10 +3002,10 @@
         <v>172</v>
       </c>
       <c r="D5">
-        <v>460</v>
+        <v>230</v>
       </c>
       <c r="E5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -2892,16 +3013,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C6">
         <v>172</v>
       </c>
       <c r="D6">
-        <v>580</v>
+        <v>290</v>
       </c>
       <c r="E6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -2909,16 +3030,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C7">
         <v>126</v>
       </c>
       <c r="D7">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -2926,16 +3047,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C8">
         <v>172</v>
       </c>
       <c r="D8">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -2943,16 +3064,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C9">
         <v>210</v>
       </c>
       <c r="D9">
-        <v>1200</v>
+        <v>600</v>
       </c>
       <c r="E9" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -2960,16 +3081,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C10">
         <v>126</v>
       </c>
       <c r="D10">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E10" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -2977,16 +3098,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C11">
         <v>172</v>
       </c>
       <c r="D11">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="E11" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3040,19 +3161,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>1837</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -3060,19 +3181,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C3">
         <v>1864</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -3080,19 +3201,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C4">
         <v>1700</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -3100,19 +3221,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>1782</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3120,19 +3241,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>1314</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3140,19 +3261,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>1221</v>
       </c>
       <c r="D7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -3160,19 +3281,19 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C8">
         <v>1250</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -3180,19 +3301,19 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C9">
         <v>1136</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -3200,19 +3321,19 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>1890</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3220,19 +3341,19 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <v>1139</v>
       </c>
       <c r="D11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3240,19 +3361,19 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C12">
         <v>1604</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -3260,19 +3381,19 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C13">
         <v>1734</v>
       </c>
       <c r="D13" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3280,19 +3401,19 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C14">
         <v>1965</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -3300,19 +3421,19 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C15">
         <v>1407</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F15" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -3320,19 +3441,19 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C16">
         <v>1479</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3340,19 +3461,19 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C17">
         <v>1290</v>
       </c>
       <c r="D17" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -3360,19 +3481,19 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C18">
         <v>1266</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E18" t="s">
         <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -3380,19 +3501,19 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C19">
         <v>1547</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
       </c>
       <c r="F19" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -3400,19 +3521,19 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C20">
         <v>1583</v>
       </c>
       <c r="D20" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -3420,19 +3541,19 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C21">
         <v>1231</v>
       </c>
       <c r="D21" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -3440,19 +3561,19 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C22">
         <v>1462</v>
       </c>
       <c r="D22" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -3460,19 +3581,19 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C23">
         <v>1149</v>
       </c>
       <c r="D23" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
       </c>
       <c r="F23" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3480,19 +3601,19 @@
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C24">
         <v>1682</v>
       </c>
       <c r="D24" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E24" t="s">
         <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3500,19 +3621,19 @@
         <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C25">
         <v>1924</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -3520,19 +3641,19 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C26">
         <v>1004</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -3540,19 +3661,19 @@
         <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C27">
         <v>1424</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -3560,19 +3681,19 @@
         <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C28">
         <v>1480</v>
       </c>
       <c r="D28" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E28" t="s">
         <v>16</v>
       </c>
       <c r="F28" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -3580,19 +3701,19 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C29">
         <v>1386</v>
       </c>
       <c r="D29" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3600,19 +3721,19 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C30">
         <v>1998</v>
       </c>
       <c r="D30" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E30" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F30" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3620,19 +3741,19 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C31">
         <v>1433</v>
       </c>
       <c r="D31" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3640,19 +3761,19 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C32">
         <v>1972</v>
       </c>
       <c r="D32" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
       </c>
       <c r="F32" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -3660,19 +3781,19 @@
         <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C33">
         <v>1508</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E33" t="s">
         <v>16</v>
       </c>
       <c r="F33" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -3680,19 +3801,19 @@
         <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C34">
         <v>1673</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
       </c>
       <c r="F34" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -3700,19 +3821,19 @@
         <v>23</v>
       </c>
       <c r="B35" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C35">
         <v>1916</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -3720,19 +3841,19 @@
         <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C36">
         <v>1768</v>
       </c>
       <c r="D36" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>
       </c>
       <c r="F36" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3740,19 +3861,19 @@
         <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C37">
         <v>1285</v>
       </c>
       <c r="D37" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E37" t="s">
         <v>15</v>
       </c>
       <c r="F37" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3760,19 +3881,19 @@
         <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C38">
         <v>1465</v>
       </c>
       <c r="D38" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
       </c>
       <c r="F38" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -3780,19 +3901,19 @@
         <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C39">
         <v>1832</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E39" t="s">
         <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -3800,19 +3921,19 @@
         <v>26</v>
       </c>
       <c r="B40" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C40">
         <v>1385</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
       </c>
       <c r="F40" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -3820,19 +3941,19 @@
         <v>27</v>
       </c>
       <c r="B41" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C41">
         <v>1118</v>
       </c>
       <c r="D41" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -3840,19 +3961,19 @@
         <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C42">
         <v>1641</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
       </c>
       <c r="F42" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3860,19 +3981,19 @@
         <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C43">
         <v>1325</v>
       </c>
       <c r="D43" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E43" t="s">
         <v>16</v>
       </c>
       <c r="F43" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -3880,19 +4001,19 @@
         <v>29</v>
       </c>
       <c r="B44" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C44">
         <v>1620</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E44" t="s">
         <v>16</v>
       </c>
       <c r="F44" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -3900,19 +4021,19 @@
         <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C45">
         <v>1518</v>
       </c>
       <c r="D45" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
       </c>
       <c r="F45" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -3920,19 +4041,19 @@
         <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C46">
         <v>1783</v>
       </c>
       <c r="D46" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E46" t="s">
         <v>13</v>
       </c>
       <c r="F46" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -3940,19 +4061,19 @@
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C47">
         <v>1162</v>
       </c>
       <c r="D47" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
       </c>
       <c r="F47" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -3960,19 +4081,19 @@
         <v>33</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C48">
         <v>1557</v>
       </c>
       <c r="D48" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E48" t="s">
         <v>15</v>
       </c>
       <c r="F48" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -3980,19 +4101,19 @@
         <v>33</v>
       </c>
       <c r="B49" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C49">
         <v>1411</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E49" t="s">
         <v>15</v>
       </c>
       <c r="F49" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -4000,19 +4121,19 @@
         <v>34</v>
       </c>
       <c r="B50" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C50">
         <v>1866</v>
       </c>
       <c r="D50" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E50" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F50" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -4020,19 +4141,19 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C51">
         <v>1116</v>
       </c>
       <c r="D51" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E51" t="s">
         <v>16</v>
       </c>
       <c r="F51" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -4040,19 +4161,19 @@
         <v>36</v>
       </c>
       <c r="B52" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C52">
         <v>1158</v>
       </c>
       <c r="D52" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E52" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F52" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -4060,19 +4181,19 @@
         <v>36</v>
       </c>
       <c r="B53" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C53">
         <v>1158</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>
       </c>
       <c r="F53" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -4080,19 +4201,19 @@
         <v>37</v>
       </c>
       <c r="B54" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C54">
         <v>1314</v>
       </c>
       <c r="D54" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E54" t="s">
         <v>13</v>
       </c>
       <c r="F54" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -4100,19 +4221,19 @@
         <v>38</v>
       </c>
       <c r="B55" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C55">
         <v>1221</v>
       </c>
       <c r="D55" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E55" t="s">
         <v>16</v>
       </c>
       <c r="F55" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -4120,19 +4241,19 @@
         <v>38</v>
       </c>
       <c r="B56" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C56">
         <v>1139</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E56" t="s">
         <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
@@ -4140,19 +4261,19 @@
         <v>39</v>
       </c>
       <c r="B57" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C57">
         <v>1965</v>
       </c>
       <c r="D57" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E57" t="s">
         <v>13</v>
       </c>
       <c r="F57" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -4160,19 +4281,19 @@
         <v>40</v>
       </c>
       <c r="B58" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C58">
         <v>2018</v>
       </c>
       <c r="D58" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E58" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F58" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -4180,19 +4301,19 @@
         <v>41</v>
       </c>
       <c r="B59" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C59">
         <v>1534</v>
       </c>
       <c r="D59" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E59" t="s">
         <v>14</v>
       </c>
       <c r="F59" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -4200,19 +4321,19 @@
         <v>40</v>
       </c>
       <c r="B60" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C60">
         <v>1290</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E60" t="s">
         <v>13</v>
       </c>
       <c r="F60" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -4220,19 +4341,19 @@
         <v>41</v>
       </c>
       <c r="B61" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C61">
         <v>1682</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
       </c>
       <c r="F61" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -4240,19 +4361,19 @@
         <v>42</v>
       </c>
       <c r="B62" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C62">
         <v>1924</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E62" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F62" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -4260,19 +4381,19 @@
         <v>43</v>
       </c>
       <c r="B63" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C63">
         <v>1744</v>
       </c>
       <c r="D63" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
       </c>
       <c r="F63" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -4280,19 +4401,19 @@
         <v>44</v>
       </c>
       <c r="B64" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C64">
         <v>1209</v>
       </c>
       <c r="D64" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E64" t="s">
         <v>15</v>
       </c>
       <c r="F64" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -4300,19 +4421,19 @@
         <v>45</v>
       </c>
       <c r="B65" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C65">
         <v>1321</v>
       </c>
       <c r="D65" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E65" t="s">
         <v>15</v>
       </c>
       <c r="F65" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -4320,19 +4441,19 @@
         <v>46</v>
       </c>
       <c r="B66" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C66">
         <v>1649</v>
       </c>
       <c r="D66" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E66" t="s">
         <v>15</v>
       </c>
       <c r="F66" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -4340,19 +4461,19 @@
         <v>43</v>
       </c>
       <c r="B67" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C67">
         <v>1998</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E67" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F67" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
@@ -4360,19 +4481,19 @@
         <v>44</v>
       </c>
       <c r="B68" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C68">
         <v>1433</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E68" t="s">
         <v>13</v>
       </c>
       <c r="F68" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
@@ -4380,19 +4501,19 @@
         <v>45</v>
       </c>
       <c r="B69" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C69">
         <v>1972</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E69" t="s">
         <v>15</v>
       </c>
       <c r="F69" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
@@ -4400,19 +4521,19 @@
         <v>46</v>
       </c>
       <c r="B70" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C70">
         <v>1285</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
       </c>
       <c r="F70" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
@@ -4420,19 +4541,19 @@
         <v>47</v>
       </c>
       <c r="B71" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C71">
         <v>1465</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E71" t="s">
         <v>15</v>
       </c>
       <c r="F71" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
@@ -4440,19 +4561,19 @@
         <v>48</v>
       </c>
       <c r="B72" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C72">
         <v>1325</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E72" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F72" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -4460,19 +4581,19 @@
         <v>49</v>
       </c>
       <c r="B73" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C73">
         <v>1600</v>
       </c>
       <c r="D73" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E73" t="s">
         <v>14</v>
       </c>
       <c r="F73" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -4480,19 +4601,19 @@
         <v>49</v>
       </c>
       <c r="B74" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C74">
         <v>1557</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E74" t="s">
         <v>13</v>
       </c>
       <c r="F74" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
@@ -4500,19 +4621,19 @@
         <v>50</v>
       </c>
       <c r="B75" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C75">
         <v>1221</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E75" t="s">
         <v>15</v>
       </c>
       <c r="F75" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -4536,7 +4657,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4562,10 +4683,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>263</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -4574,10 +4695,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>262</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -4586,10 +4707,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>259</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -4598,10 +4719,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>260</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -4610,10 +4731,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix DataBase + Create new combos for the scatterplot
</commit_message>
<xml_diff>
--- a/Work/Data/db.xlsx
+++ b/Work/Data/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\PyProject\python_project_192\Work\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FEF909-85C5-401E-B098-82EC63EC9DED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0850B710-89DB-456A-91CF-40CE8D32969D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3E971001-3800-4193-8498-245E767CB2F4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{3E971001-3800-4193-8498-245E767CB2F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Учет" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Отдел" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Информация!$A$1:$F$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Информация!$A$1:$F$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Работник!$A$1:$C$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Учет!$A$1:$E$51</definedName>
   </definedNames>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="189">
   <si>
     <t>Код</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Высшее</t>
   </si>
   <si>
-    <t>Среднее общее</t>
-  </si>
-  <si>
     <t>Среднее профессиональное</t>
   </si>
   <si>
@@ -104,30 +101,12 @@
     <t>Бухгалтер</t>
   </si>
   <si>
-    <t>Павлов Евдоким Валерьянович</t>
-  </si>
-  <si>
     <t>Трофимов Платон Семенович</t>
   </si>
   <si>
-    <t>Шестаков Самуил Тимурович</t>
-  </si>
-  <si>
-    <t>Пестов Алексей Иринеевич</t>
-  </si>
-  <si>
     <t>Суханова Наталья Евсеевна</t>
   </si>
   <si>
-    <t>Лазарев Елисей Гордеевич</t>
-  </si>
-  <si>
-    <t>Суханова Амелия Тимофеевна</t>
-  </si>
-  <si>
-    <t>Зуев Феликс Георгьевич</t>
-  </si>
-  <si>
     <t>Зыкова Женевьева Тимофеевна</t>
   </si>
   <si>
@@ -137,171 +116,42 @@
     <t>Белоусов Арсений Оскарович</t>
   </si>
   <si>
-    <t>Щербаков Вадим Вадимович</t>
-  </si>
-  <si>
-    <t>Комаров Валерий Геннадиевич</t>
-  </si>
-  <si>
     <t>Зыков Петр Давидович</t>
   </si>
   <si>
-    <t>Савельев Панкрат Григорьевич</t>
-  </si>
-  <si>
-    <t>Борисова Эмилия Борисовна</t>
-  </si>
-  <si>
-    <t>Баранов Геннадий Филиппович</t>
-  </si>
-  <si>
-    <t>Коновалов Петр Иринеевич</t>
-  </si>
-  <si>
-    <t>Брагин Лукьян Онисимович</t>
-  </si>
-  <si>
     <t>Евсеев Демьян Антонович</t>
   </si>
   <si>
-    <t>Мишин Тимур Сергеевич</t>
-  </si>
-  <si>
     <t>Сысоев Захар Русланович</t>
   </si>
   <si>
-    <t>Аксёнов Гарри Глебович</t>
-  </si>
-  <si>
-    <t>Костин Денис Парфеньевич</t>
-  </si>
-  <si>
-    <t>Блинова Риана Руслановна</t>
-  </si>
-  <si>
-    <t>Третьяков Нелли Платонович</t>
-  </si>
-  <si>
-    <t>Николаев Панкрат Львович</t>
-  </si>
-  <si>
     <t>Горбунов Артур Иванович</t>
   </si>
   <si>
-    <t>Лукин Юстиниан Онисимович</t>
-  </si>
-  <si>
-    <t>Архипов Руслан Адольфович</t>
-  </si>
-  <si>
-    <t>Носков Василий Федорович</t>
-  </si>
-  <si>
-    <t>Королёв Карл Валентинович</t>
-  </si>
-  <si>
-    <t>Марков Аверкий Степанович</t>
-  </si>
-  <si>
-    <t>Hidden Bluff Cove, Shaktoolik, ND</t>
-  </si>
-  <si>
-    <t>Burning Beacon Ramp, Iron Horse</t>
-  </si>
-  <si>
-    <t>Stony Sky Run, You Bet</t>
-  </si>
-  <si>
-    <t>Iron Canyon, Bullfrog, OR, 97710-4707</t>
-  </si>
-  <si>
-    <t>Red Wagon Heights, Dixie, AR</t>
-  </si>
-  <si>
     <t>Jagged Gate, Toppenish, WY, 82526-8820</t>
   </si>
   <si>
-    <t>Silent Gate Crest, Usk, NH</t>
-  </si>
-  <si>
     <t>Bright Expressway, Gay, LA, 71318-1559</t>
   </si>
   <si>
-    <t>Cinder Mountain Meadow, Zoar, ON</t>
-  </si>
-  <si>
-    <t>Gentle Bear Cape, Lucky, SD</t>
-  </si>
-  <si>
     <t>Noble Vale, Peru, KS, 67126-0526</t>
   </si>
   <si>
-    <t>Clear Autumn Pathway, Agenda, MT</t>
-  </si>
-  <si>
-    <t>Golden Lake Forest, Ringo, DE</t>
-  </si>
-  <si>
-    <t>Merry Cloud Lookout, Paducah, ND</t>
-  </si>
-  <si>
     <t>Lazy Plaza, Tyewhoppety, TN, 38526-7920</t>
   </si>
   <si>
-    <t>Heather Common, Dry Prong, KS</t>
-  </si>
-  <si>
-    <t>Crystal Road, Blackduck, BC, V2L-5C7</t>
-  </si>
-  <si>
     <t>Velvet Line, Ottertail, ME, 04747-1131</t>
   </si>
   <si>
-    <t>Foggy Creek Maze, Jerktail, TX</t>
-  </si>
-  <si>
-    <t>Sunny Pioneer Green, Wamduska, MI</t>
-  </si>
-  <si>
     <t>Quiet Trace, Bushnell, IN, 46213-3328</t>
   </si>
   <si>
-    <t>Dusty Point, Montreal, WI, 54473-1297</t>
-  </si>
-  <si>
-    <t>Harvest Avenue, Crackertown, MI, 48802-0974</t>
-  </si>
-  <si>
-    <t>Hazy Rise Autoroute, Thunderbolt, MO</t>
-  </si>
-  <si>
-    <t>Cotton Goose Turnabout, Monumental, NE</t>
-  </si>
-  <si>
-    <t>Amber Apple Wharf, Sunshine, ME</t>
-  </si>
-  <si>
     <t>Umber Street, Timberlost, NE, 69698-9165</t>
   </si>
   <si>
-    <t>Colonial Mountain, Paulins Kill, DE</t>
-  </si>
-  <si>
-    <t>Round Prairie Landing, Great Kills</t>
-  </si>
-  <si>
-    <t>Dewy Dale, Matrimony, MB, R1Q-8X1</t>
-  </si>
-  <si>
-    <t>Grand Butterfly Freeway, Perfection, ON</t>
-  </si>
-  <si>
     <t>Emerald Pike, Sharpeye, WY, 83158-2929</t>
   </si>
   <si>
-    <t>Shady Towers, Whisler, WY, 83101-4037</t>
-  </si>
-  <si>
     <t>Wishing Close, Pilltown, LA, 70482-3691</t>
   </si>
   <si>
@@ -314,9 +164,6 @@
     <t>+7(495)824-74-13</t>
   </si>
   <si>
-    <t>+7(495)394-22-70</t>
-  </si>
-  <si>
     <t>+7(495)968-68-48</t>
   </si>
   <si>
@@ -326,9 +173,6 @@
     <t>+7(495)415-83-97</t>
   </si>
   <si>
-    <t>+7(495)828-10-92</t>
-  </si>
-  <si>
     <t>+7(495)606-45-43</t>
   </si>
   <si>
@@ -344,114 +188,48 @@
     <t>+7(495)268-70-27</t>
   </si>
   <si>
-    <t>+7(495)778-44-45</t>
-  </si>
-  <si>
     <t>+7(495)646-62-55</t>
   </si>
   <si>
-    <t>+7(495)252-08-24</t>
-  </si>
-  <si>
-    <t>+7(495)838-95-69</t>
-  </si>
-  <si>
-    <t>+7(495)387-83-22</t>
-  </si>
-  <si>
-    <t>+7(495)796-94-12</t>
-  </si>
-  <si>
-    <t>+7(495)747-56-16</t>
-  </si>
-  <si>
-    <t>+7(495)455-01-44</t>
-  </si>
-  <si>
-    <t>+7(495)314-73-76</t>
-  </si>
-  <si>
-    <t>+7(495)631-04-38</t>
-  </si>
-  <si>
-    <t>+7(495)857-57-40</t>
-  </si>
-  <si>
     <t>+7(495)953-10-76</t>
   </si>
   <si>
-    <t>+7(495)811-28-84</t>
-  </si>
-  <si>
     <t>+7(495)155-69-48</t>
   </si>
   <si>
-    <t>+7(495)962-71-39</t>
-  </si>
-  <si>
     <t>+7(495)931-00-84</t>
   </si>
   <si>
     <t>+7(495)961-85-53</t>
   </si>
   <si>
-    <t>+7(916)424-30-91</t>
-  </si>
-  <si>
     <t>+7(916)897-19-45</t>
   </si>
   <si>
-    <t>+7(916)960-73-39</t>
-  </si>
-  <si>
     <t>+7(916)630-63-27</t>
   </si>
   <si>
-    <t>+7(916)511-60-23</t>
-  </si>
-  <si>
     <t>+7(916)100-15-69</t>
   </si>
   <si>
     <t>+7(916)291-63-13</t>
   </si>
   <si>
-    <t>+7(916)446-76-45</t>
-  </si>
-  <si>
     <t>+7(916)568-69-15</t>
   </si>
   <si>
     <t>+7(916)262-72-11</t>
   </si>
   <si>
-    <t>+7(952)756-17-22</t>
-  </si>
-  <si>
     <t>+7(952)850-72-13</t>
   </si>
   <si>
-    <t>+7(952)687-19-01</t>
-  </si>
-  <si>
     <t>+7(952)818-31-15</t>
   </si>
   <si>
     <t>+7(952)720-55-36</t>
   </si>
   <si>
-    <t>+7(952)860-08-46</t>
-  </si>
-  <si>
-    <t>+7(952)237-24-96</t>
-  </si>
-  <si>
-    <t>+7(952)056-17-20</t>
-  </si>
-  <si>
-    <t>+7(952)510-04-64</t>
-  </si>
-  <si>
     <t>+7(952)354-20-08</t>
   </si>
   <si>
@@ -500,12 +278,6 @@
     <t>Норма (ч/мес)</t>
   </si>
   <si>
-    <t>Высшее/Среднее профессиональное</t>
-  </si>
-  <si>
-    <t>Высшее/Неоконченное высшее/Студент</t>
-  </si>
-  <si>
     <t>Пономарев Богдан Викторович</t>
   </si>
   <si>
@@ -834,6 +606,9 @@
   </si>
   <si>
     <t>Обучение</t>
+  </si>
+  <si>
+    <t>Sunny Pioneer Green, Wamduska, MI, 15786-3482</t>
   </si>
 </sst>
 </file>
@@ -1281,7 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802CA84B-12BF-4C23-A805-60116DA63581}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1300,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2911,10 +2686,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C78A7D8-24EA-4D09-A2F0-CA9351E1F58B}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2925,7 +2700,7 @@
     <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2933,18 +2708,18 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>172</v>
@@ -2952,17 +2727,14 @@
       <c r="D2">
         <v>900</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>71</v>
       </c>
       <c r="C3">
         <v>172</v>
@@ -2970,16 +2742,13 @@
       <c r="D3">
         <v>800</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>172</v>
@@ -2987,16 +2756,13 @@
       <c r="D4">
         <v>175</v>
       </c>
-      <c r="E4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>172</v>
@@ -3004,16 +2770,13 @@
       <c r="D5">
         <v>230</v>
       </c>
-      <c r="E5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>144</v>
+        <v>70</v>
       </c>
       <c r="C6">
         <v>172</v>
@@ -3021,16 +2784,13 @@
       <c r="D6">
         <v>290</v>
       </c>
-      <c r="E6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="C7">
         <v>126</v>
@@ -3038,16 +2798,13 @@
       <c r="D7">
         <v>400</v>
       </c>
-      <c r="E7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>73</v>
       </c>
       <c r="C8">
         <v>172</v>
@@ -3055,16 +2812,13 @@
       <c r="D8">
         <v>500</v>
       </c>
-      <c r="E8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="C9">
         <v>210</v>
@@ -3072,16 +2826,13 @@
       <c r="D9">
         <v>600</v>
       </c>
-      <c r="E9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>75</v>
       </c>
       <c r="C10">
         <v>126</v>
@@ -3089,25 +2840,19 @@
       <c r="D10">
         <v>350</v>
       </c>
-      <c r="E10" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>76</v>
       </c>
       <c r="C11">
         <v>172</v>
       </c>
       <c r="D11">
         <v>250</v>
-      </c>
-      <c r="E11" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3119,10 +2864,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9A834C-B529-4046-AC5D-6954E484C53A}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3156,1496 +2901,1016 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="C2">
-        <v>1837</v>
-      </c>
-      <c r="D2" t="s">
-        <v>105</v>
+        <v>1864</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
       <c r="C3">
-        <v>1864</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>155</v>
+        <v>1700</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>156</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>1700</v>
+        <v>1782</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>160</v>
       </c>
       <c r="C5">
-        <v>1782</v>
-      </c>
-      <c r="D5" t="s">
-        <v>123</v>
+        <v>1250</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>162</v>
       </c>
       <c r="C6">
-        <v>1314</v>
-      </c>
-      <c r="D6" t="s">
-        <v>94</v>
+        <v>1136</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>1221</v>
+        <v>1890</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>236</v>
+        <v>163</v>
       </c>
       <c r="C8">
-        <v>1250</v>
+        <v>1604</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>213</v>
+        <v>139</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>238</v>
+        <v>84</v>
       </c>
       <c r="C9">
-        <v>1136</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>214</v>
+        <v>1734</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>196</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="C10">
-        <v>1890</v>
-      </c>
-      <c r="D10" t="s">
-        <v>89</v>
+        <v>1407</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="F10" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="C11">
-        <v>1139</v>
+        <v>1479</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>239</v>
+        <v>182</v>
       </c>
       <c r="C12">
-        <v>1604</v>
+        <v>1266</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>215</v>
+        <v>141</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>198</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>21</v>
       </c>
       <c r="C13">
-        <v>1734</v>
+        <v>1547</v>
       </c>
       <c r="D13" t="s">
-        <v>122</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="C14">
-        <v>1965</v>
+        <v>1583</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>240</v>
+        <v>22</v>
       </c>
       <c r="C15">
-        <v>1407</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>216</v>
+        <v>1231</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>91</v>
       </c>
       <c r="C16">
-        <v>1479</v>
+        <v>1462</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>1149</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
         <v>13</v>
       </c>
-      <c r="F16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
-        <v>11</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17">
-        <v>1290</v>
-      </c>
-      <c r="D17" t="s">
-        <v>107</v>
-      </c>
-      <c r="E17" t="s">
-        <v>16</v>
-      </c>
       <c r="F17" t="s">
-        <v>59</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>258</v>
+        <v>161</v>
       </c>
       <c r="C18">
-        <v>1266</v>
+        <v>1004</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>217</v>
+        <v>142</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>165</v>
       </c>
       <c r="C19">
-        <v>1547</v>
-      </c>
-      <c r="D19" t="s">
-        <v>131</v>
+        <v>1424</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
       </c>
       <c r="F19" t="s">
-        <v>200</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>85</v>
       </c>
       <c r="C20">
-        <v>1583</v>
+        <v>1480</v>
       </c>
       <c r="D20" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C21">
-        <v>1231</v>
+        <v>1386</v>
       </c>
       <c r="D21" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>201</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C22">
-        <v>1462</v>
-      </c>
-      <c r="D22" t="s">
-        <v>115</v>
+        <v>1508</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>202</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="C23">
-        <v>1149</v>
-      </c>
-      <c r="D23" t="s">
-        <v>101</v>
+        <v>1673</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
       </c>
       <c r="F23" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>168</v>
+      </c>
+      <c r="C24">
+        <v>1916</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25">
+        <v>1768</v>
+      </c>
+      <c r="D25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
         <v>31</v>
-      </c>
-      <c r="C24">
-        <v>1682</v>
-      </c>
-      <c r="D24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="4">
-        <v>18</v>
-      </c>
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25">
-        <v>1924</v>
-      </c>
-      <c r="D25" t="s">
-        <v>127</v>
-      </c>
-      <c r="E25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>237</v>
+        <v>169</v>
       </c>
       <c r="C26">
-        <v>1004</v>
+        <v>1832</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>218</v>
+        <v>147</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>204</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>241</v>
+        <v>170</v>
       </c>
       <c r="C27">
-        <v>1424</v>
+        <v>1385</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>177</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>161</v>
+        <v>93</v>
       </c>
       <c r="C28">
-        <v>1480</v>
+        <v>1118</v>
       </c>
       <c r="D28" t="s">
-        <v>136</v>
+        <v>41</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>205</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C29">
-        <v>1386</v>
+        <v>1641</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>171</v>
       </c>
       <c r="C30">
-        <v>1998</v>
-      </c>
-      <c r="D30" t="s">
-        <v>119</v>
+        <v>1620</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="E30" t="s">
-        <v>142</v>
+        <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="C31">
-        <v>1433</v>
+        <v>1518</v>
       </c>
       <c r="D31" t="s">
-        <v>133</v>
+        <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C32">
-        <v>1972</v>
+        <v>1783</v>
       </c>
       <c r="D32" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F32" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>242</v>
+        <v>94</v>
       </c>
       <c r="C33">
-        <v>1508</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>219</v>
+        <v>1162</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
       </c>
       <c r="E33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F33" t="s">
-        <v>178</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>243</v>
+        <v>181</v>
       </c>
       <c r="C34">
-        <v>1673</v>
+        <v>1411</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>221</v>
+        <v>150</v>
       </c>
       <c r="E34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F34" t="s">
-        <v>179</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>244</v>
+        <v>92</v>
       </c>
       <c r="C35">
-        <v>1916</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>222</v>
+        <v>1866</v>
+      </c>
+      <c r="D35" t="s">
+        <v>49</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="F35" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>157</v>
+        <v>97</v>
       </c>
       <c r="C36">
-        <v>1768</v>
+        <v>1116</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>172</v>
+      </c>
+      <c r="C37">
+        <v>1158</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38">
+        <v>1314</v>
+      </c>
+      <c r="D38" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" t="s">
         <v>13</v>
       </c>
-      <c r="F36" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="4">
-        <v>25</v>
-      </c>
-      <c r="B37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37">
-        <v>1285</v>
-      </c>
-      <c r="D37" t="s">
-        <v>114</v>
-      </c>
-      <c r="E37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="4">
-        <v>26</v>
-      </c>
-      <c r="B38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38">
-        <v>1465</v>
-      </c>
-      <c r="D38" t="s">
-        <v>112</v>
-      </c>
-      <c r="E38" t="s">
-        <v>15</v>
-      </c>
       <c r="F38" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>245</v>
+        <v>173</v>
       </c>
       <c r="C39">
-        <v>1832</v>
+        <v>1139</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>223</v>
+        <v>152</v>
       </c>
       <c r="E39" t="s">
         <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>181</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>246</v>
+        <v>95</v>
       </c>
       <c r="C40">
-        <v>1385</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>224</v>
+        <v>1965</v>
+      </c>
+      <c r="D40" t="s">
+        <v>54</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
       </c>
       <c r="F40" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C41">
-        <v>1118</v>
-      </c>
-      <c r="D41" t="s">
-        <v>92</v>
+        <v>1290</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>153</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
       <c r="C42">
-        <v>1641</v>
-      </c>
-      <c r="D42" t="s">
-        <v>130</v>
+        <v>1682</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>154</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
       </c>
       <c r="F42" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C43">
-        <v>1325</v>
-      </c>
-      <c r="D43" t="s">
-        <v>110</v>
+        <v>1924</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="E43" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="F43" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>247</v>
+        <v>176</v>
       </c>
       <c r="C44">
-        <v>1620</v>
+        <v>1998</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>225</v>
+        <v>155</v>
       </c>
       <c r="E44" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="F44" t="s">
-        <v>183</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C45">
-        <v>1518</v>
-      </c>
-      <c r="D45" t="s">
-        <v>93</v>
+        <v>1433</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>156</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
       </c>
       <c r="F45" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>177</v>
       </c>
       <c r="C46">
-        <v>1783</v>
-      </c>
-      <c r="D46" t="s">
-        <v>87</v>
+        <v>1972</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F46" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C47">
-        <v>1162</v>
-      </c>
-      <c r="D47" t="s">
-        <v>95</v>
+        <v>1285</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="E47" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F47" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="C48">
-        <v>1557</v>
-      </c>
-      <c r="D48" t="s">
-        <v>109</v>
+        <v>1465</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="E48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F48" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>257</v>
+        <v>88</v>
       </c>
       <c r="C49">
-        <v>1411</v>
+        <v>1325</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>226</v>
+        <v>57</v>
       </c>
       <c r="E49" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="F49" t="s">
-        <v>184</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="C50">
-        <v>1866</v>
-      </c>
-      <c r="D50" t="s">
-        <v>111</v>
+        <v>1557</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="E50" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="F50" t="s">
-        <v>208</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>173</v>
+        <v>87</v>
       </c>
       <c r="C51">
-        <v>1116</v>
-      </c>
-      <c r="D51" t="s">
-        <v>113</v>
+        <v>1221</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="E51" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F51" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="4">
         <v>36</v>
       </c>
-      <c r="B52" t="s">
-        <v>43</v>
-      </c>
-      <c r="C52">
-        <v>1158</v>
-      </c>
-      <c r="D52" t="s">
-        <v>108</v>
-      </c>
-      <c r="E52" t="s">
-        <v>142</v>
-      </c>
-      <c r="F52" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="4">
-        <v>36</v>
-      </c>
-      <c r="B53" t="s">
-        <v>248</v>
-      </c>
-      <c r="C53">
-        <v>1158</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="E53" t="s">
-        <v>15</v>
-      </c>
-      <c r="F53" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="4">
-        <v>37</v>
-      </c>
-      <c r="B54" t="s">
-        <v>158</v>
-      </c>
-      <c r="C54">
-        <v>1314</v>
-      </c>
-      <c r="D54" t="s">
-        <v>97</v>
-      </c>
-      <c r="E54" t="s">
-        <v>13</v>
-      </c>
-      <c r="F54" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="4">
-        <v>38</v>
-      </c>
-      <c r="B55" t="s">
-        <v>44</v>
-      </c>
-      <c r="C55">
-        <v>1221</v>
-      </c>
-      <c r="D55" t="s">
-        <v>100</v>
-      </c>
-      <c r="E55" t="s">
-        <v>16</v>
-      </c>
-      <c r="F55" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="4">
-        <v>38</v>
-      </c>
-      <c r="B56" t="s">
-        <v>249</v>
-      </c>
-      <c r="C56">
-        <v>1139</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="E56" t="s">
-        <v>13</v>
-      </c>
-      <c r="F56" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="4">
-        <v>39</v>
-      </c>
-      <c r="B57" t="s">
-        <v>171</v>
-      </c>
-      <c r="C57">
-        <v>1965</v>
-      </c>
-      <c r="D57" t="s">
-        <v>120</v>
-      </c>
-      <c r="E57" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="4">
-        <v>40</v>
-      </c>
-      <c r="B58" t="s">
-        <v>45</v>
-      </c>
-      <c r="C58">
-        <v>2018</v>
-      </c>
-      <c r="D58" t="s">
-        <v>121</v>
-      </c>
-      <c r="E58" t="s">
-        <v>142</v>
-      </c>
-      <c r="F58" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="4">
-        <v>41</v>
-      </c>
-      <c r="B59" t="s">
-        <v>46</v>
-      </c>
-      <c r="C59">
-        <v>1534</v>
-      </c>
-      <c r="D59" t="s">
-        <v>117</v>
-      </c>
-      <c r="E59" t="s">
-        <v>14</v>
-      </c>
-      <c r="F59" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" s="4">
-        <v>40</v>
-      </c>
-      <c r="B60" t="s">
-        <v>250</v>
-      </c>
-      <c r="C60">
-        <v>1290</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="E60" t="s">
-        <v>13</v>
-      </c>
-      <c r="F60" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="4">
-        <v>41</v>
-      </c>
-      <c r="B61" t="s">
-        <v>251</v>
-      </c>
-      <c r="C61">
-        <v>1682</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="E61" t="s">
-        <v>13</v>
-      </c>
-      <c r="F61" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="4">
-        <v>42</v>
-      </c>
-      <c r="B62" t="s">
-        <v>47</v>
-      </c>
-      <c r="C62">
-        <v>1924</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E62" t="s">
-        <v>142</v>
-      </c>
-      <c r="F62" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="4">
-        <v>43</v>
-      </c>
-      <c r="B63" t="s">
-        <v>48</v>
-      </c>
-      <c r="C63">
-        <v>1744</v>
-      </c>
-      <c r="D63" t="s">
-        <v>132</v>
-      </c>
-      <c r="E63" t="s">
-        <v>15</v>
-      </c>
-      <c r="F63" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="4">
-        <v>44</v>
-      </c>
-      <c r="B64" t="s">
-        <v>49</v>
-      </c>
-      <c r="C64">
-        <v>1209</v>
-      </c>
-      <c r="D64" t="s">
-        <v>106</v>
-      </c>
-      <c r="E64" t="s">
-        <v>15</v>
-      </c>
-      <c r="F64" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="4">
-        <v>45</v>
-      </c>
-      <c r="B65" t="s">
-        <v>50</v>
-      </c>
-      <c r="C65">
-        <v>1321</v>
-      </c>
-      <c r="D65" t="s">
-        <v>102</v>
-      </c>
-      <c r="E65" t="s">
-        <v>15</v>
-      </c>
-      <c r="F65" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="4">
-        <v>46</v>
-      </c>
-      <c r="B66" t="s">
-        <v>51</v>
-      </c>
-      <c r="C66">
-        <v>1649</v>
-      </c>
-      <c r="D66" t="s">
-        <v>134</v>
-      </c>
-      <c r="E66" t="s">
-        <v>15</v>
-      </c>
-      <c r="F66" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="4">
-        <v>43</v>
-      </c>
-      <c r="B67" t="s">
-        <v>252</v>
-      </c>
-      <c r="C67">
-        <v>1998</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="E67" t="s">
-        <v>142</v>
-      </c>
-      <c r="F67" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" s="4">
-        <v>44</v>
-      </c>
-      <c r="B68" t="s">
-        <v>254</v>
-      </c>
-      <c r="C68">
-        <v>1433</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="E68" t="s">
-        <v>13</v>
-      </c>
-      <c r="F68" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="4">
-        <v>45</v>
-      </c>
-      <c r="B69" t="s">
-        <v>253</v>
-      </c>
-      <c r="C69">
-        <v>1972</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="E69" t="s">
-        <v>15</v>
-      </c>
-      <c r="F69" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="4">
-        <v>46</v>
-      </c>
-      <c r="B70" t="s">
-        <v>255</v>
-      </c>
-      <c r="C70">
-        <v>1285</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="E70" t="s">
-        <v>13</v>
-      </c>
-      <c r="F70" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="4">
-        <v>47</v>
-      </c>
-      <c r="B71" t="s">
-        <v>172</v>
-      </c>
-      <c r="C71">
-        <v>1465</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E71" t="s">
-        <v>15</v>
-      </c>
-      <c r="F71" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="4">
-        <v>48</v>
-      </c>
-      <c r="B72" t="s">
-        <v>164</v>
-      </c>
-      <c r="C72">
-        <v>1325</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E72" t="s">
-        <v>142</v>
-      </c>
-      <c r="F72" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="4">
-        <v>49</v>
-      </c>
-      <c r="B73" t="s">
-        <v>52</v>
-      </c>
-      <c r="C73">
-        <v>1600</v>
-      </c>
-      <c r="D73" t="s">
-        <v>135</v>
-      </c>
-      <c r="E73" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="4">
-        <v>49</v>
-      </c>
-      <c r="B74" t="s">
-        <v>256</v>
-      </c>
-      <c r="C74">
-        <v>1557</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="E74" t="s">
-        <v>13</v>
-      </c>
-      <c r="F74" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="4">
-        <v>50</v>
-      </c>
-      <c r="B75" t="s">
-        <v>163</v>
-      </c>
-      <c r="C75">
-        <v>1221</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E75" t="s">
-        <v>15</v>
-      </c>
-      <c r="F75" t="s">
-        <v>86</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F75" xr:uid="{BC7C2BAA-FB9B-4DAD-A1A8-C66F82305779}">
+  <autoFilter ref="A1:F51" xr:uid="{BC7C2BAA-FB9B-4DAD-A1A8-C66F82305779}">
     <filterColumn colId="4">
       <filters>
         <filter val="Высшее"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C82:D131">
-    <sortCondition ref="D82"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C58:D107">
+    <sortCondition ref="D58"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4683,10 +3948,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -4695,10 +3960,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>262</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -4707,10 +3972,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>259</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -4719,10 +3984,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>260</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -4731,10 +3996,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>261</v>
+        <v>185</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made Scaterplot + some fixes
</commit_message>
<xml_diff>
--- a/Work/Data/db.xlsx
+++ b/Work/Data/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\PyProject\python_project_192\Work\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0850B710-89DB-456A-91CF-40CE8D32969D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC0A978-A33A-4DB5-A4E0-285A3E6E9734}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{3E971001-3800-4193-8498-245E767CB2F4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{3E971001-3800-4193-8498-245E767CB2F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Учет" sheetId="1" r:id="rId1"/>
@@ -639,7 +639,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -682,6 +682,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -710,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -735,6 +741,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1056,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802CA84B-12BF-4C23-A805-60116DA63581}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1098,7 +1105,7 @@
       <c r="C2">
         <v>27</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="16">
         <v>60400</v>
       </c>
       <c r="E2">
@@ -1215,7 +1222,7 @@
       <c r="C8">
         <v>19</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="16">
         <v>53600</v>
       </c>
       <c r="E8">
@@ -1235,7 +1242,7 @@
       <c r="C9">
         <v>24</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="16">
         <v>51200</v>
       </c>
       <c r="E9">
@@ -1349,7 +1356,7 @@
       <c r="C15">
         <v>22</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="16">
         <v>50400</v>
       </c>
       <c r="E15">
@@ -1577,7 +1584,7 @@
       <c r="C27">
         <v>23</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="16">
         <v>56400</v>
       </c>
       <c r="E27">
@@ -2055,8 +2062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E65D3C7-96B9-4249-84BC-8FFE97811FCF}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2293,7 +2300,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
+      <c r="A20" s="16">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -2414,7 +2421,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="4">
+      <c r="A30" s="16">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
@@ -2438,7 +2445,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="4">
+      <c r="A32" s="16">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
@@ -2486,7 +2493,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="4">
+      <c r="A36" s="16">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
@@ -2582,7 +2589,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="4">
+      <c r="A44" s="16">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
@@ -2866,7 +2873,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -3922,7 +3929,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>